<commit_message>
tasks v1 TODO : other group members, dates
</commit_message>
<xml_diff>
--- a/Deliverables/Tasks.xlsx
+++ b/Deliverables/Tasks.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
-  <si>
-    <t>Tasks waiting to be completed:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="67">
   <si>
     <t>Worked by:</t>
   </si>
@@ -69,16 +66,157 @@
     <t>Week 1</t>
   </si>
   <si>
-    <t>Daniel</t>
-  </si>
-  <si>
-    <t>Something</t>
-  </si>
-  <si>
-    <t>Georgi  Ilia  Yu  Daniel</t>
-  </si>
-  <si>
-    <t>dd.mm. || hh:mm</t>
+    <t>Task:</t>
+  </si>
+  <si>
+    <t>URS v1 use cases</t>
+  </si>
+  <si>
+    <t>20.11. || 16:30</t>
+  </si>
+  <si>
+    <t>URS v1 introduction</t>
+  </si>
+  <si>
+    <t>20.11. || 16:25</t>
+  </si>
+  <si>
+    <t>URS v1 GUI</t>
+  </si>
+  <si>
+    <t>URS v1 NonFunctional</t>
+  </si>
+  <si>
+    <t>Des Doc Final sequence diagrams</t>
+  </si>
+  <si>
+    <t>Design Doc Final class diagram</t>
+  </si>
+  <si>
+    <t>Ilia, Georgi</t>
+  </si>
+  <si>
+    <t>App: Collision detection</t>
+  </si>
+  <si>
+    <t>URS v2 use cases</t>
+  </si>
+  <si>
+    <t>URS v2 NonFunctional</t>
+  </si>
+  <si>
+    <t>URS final use cases</t>
+  </si>
+  <si>
+    <t>URS final GUI</t>
+  </si>
+  <si>
+    <t>02.12. || 8:30</t>
+  </si>
+  <si>
+    <t>01.12. || 12:00</t>
+  </si>
+  <si>
+    <t>App: Path optimization</t>
+  </si>
+  <si>
+    <t>App:Process Flow</t>
+  </si>
+  <si>
+    <t>App:Prevent circular</t>
+  </si>
+  <si>
+    <t>App: Flow Out-Int</t>
+  </si>
+  <si>
+    <t>App:Max Flow Capacity</t>
+  </si>
+  <si>
+    <t>App: Pipe Safety Limit</t>
+  </si>
+  <si>
+    <t>App: Edit Pump</t>
+  </si>
+  <si>
+    <t>App: Edit Adjustable</t>
+  </si>
+  <si>
+    <t>App: Edit Pipe</t>
+  </si>
+  <si>
+    <t>App: Colored Icons</t>
+  </si>
+  <si>
+    <t>App: Undo/Redo</t>
+  </si>
+  <si>
+    <t>App:Add Element</t>
+  </si>
+  <si>
+    <t>App: Remove element</t>
+  </si>
+  <si>
+    <t>App: Add connection</t>
+  </si>
+  <si>
+    <t>App: Remove connection</t>
+  </si>
+  <si>
+    <t>App: Drag Element</t>
+  </si>
+  <si>
+    <t>App: Add Midpoint</t>
+  </si>
+  <si>
+    <t>App: Drag Midpoint</t>
+  </si>
+  <si>
+    <t>App: Remove Midpoint</t>
+  </si>
+  <si>
+    <t>App: RightClick menu</t>
+  </si>
+  <si>
+    <t>App: On Hover</t>
+  </si>
+  <si>
+    <t>App: Show Flow over Path</t>
+  </si>
+  <si>
+    <t>App: Show Flow at Sink</t>
+  </si>
+  <si>
+    <t>App: Information box</t>
+  </si>
+  <si>
+    <t>App: Save</t>
+  </si>
+  <si>
+    <t>App: Load</t>
+  </si>
+  <si>
+    <t>App:New</t>
+  </si>
+  <si>
+    <t>App:Redraw Optimization</t>
+  </si>
+  <si>
+    <t>App: Draw path</t>
+  </si>
+  <si>
+    <t>02.01. || 11:20</t>
+  </si>
+  <si>
+    <t>App: Final Edit</t>
+  </si>
+  <si>
+    <t>02.01. || 11:30</t>
+  </si>
+  <si>
+    <t>Design Doc: Documentation</t>
+  </si>
+  <si>
+    <t>09.12 || 12:30</t>
   </si>
 </sst>
 </file>
@@ -153,7 +291,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -398,40 +536,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="mediumDashed">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="mediumDashed">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -449,9 +559,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -504,18 +611,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -823,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -841,33 +936,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="C1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="D1" s="24" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>3</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="18" t="s">
+      <c r="K1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="L1" s="19" t="s">
         <v>6</v>
-      </c>
-      <c r="L1" s="20" t="s">
-        <v>7</v>
       </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -879,189 +974,654 @@
     </row>
     <row r="2" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>20</v>
-      </c>
       <c r="D2" s="6">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="17">
+      <c r="K2" s="16">
         <f>(SUMIF(B:B, "*"&amp;J2&amp;"*",D:D ))</f>
-        <v>100</v>
-      </c>
-      <c r="L2" s="30" t="str">
+        <v>85</v>
+      </c>
+      <c r="L2" s="25" t="str">
         <f>ROUNDDOWN((K2)/60,0) &amp;":"&amp;(IF(MOD(K2, 60) &lt; 10, "0","")) &amp; MOD(K2,60)</f>
-        <v>1:40</v>
-      </c>
-      <c r="M2" s="12" t="str">
-        <f>ROUND((K2) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>20%</v>
+        <v>1:25</v>
+      </c>
+      <c r="M2" s="11" t="str">
+        <f>ROUND((K2) / ($K$6), 2) * 100 &amp;"%"</f>
+        <v>14%</v>
       </c>
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="6">
-        <v>100</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="6"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I3" s="1"/>
-      <c r="J3" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="17">
-        <f t="shared" ref="K3:K5" si="0">(SUMIF(B:B, "*"&amp;J3&amp;"*",D:D ))</f>
-        <v>100</v>
-      </c>
-      <c r="L3" s="30" t="str">
-        <f t="shared" ref="L3:L5" si="1">ROUNDDOWN((K3)/60,0) &amp;":"&amp;(IF(MOD(K3, 60) &lt; 10, "0","")) &amp; MOD(K3,60)</f>
-        <v>1:40</v>
-      </c>
-      <c r="M3" s="12" t="str">
-        <f t="shared" ref="M3:M6" si="2">ROUND((K3) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>20%</v>
+      <c r="J3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="16">
+        <f>(SUMIF(B:B, "*"&amp;J3&amp;"*",D:D ))</f>
+        <v>513</v>
+      </c>
+      <c r="L3" s="25" t="str">
+        <f t="shared" ref="L3:L4" si="0">ROUNDDOWN((K3)/60,0) &amp;":"&amp;(IF(MOD(K3, 60) &lt; 10, "0","")) &amp; MOD(K3,60)</f>
+        <v>8:33</v>
+      </c>
+      <c r="M3" s="11" t="str">
+        <f>ROUND((K3) / ($K$6), 2) * 100 &amp;"%"</f>
+        <v>86%</v>
       </c>
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="21"/>
+      <c r="A4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="20"/>
       <c r="D4" s="6"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="9"/>
+      <c r="H4" s="8"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="17">
+      <c r="J4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="16">
+        <f>(SUMIF(B:B, "*"&amp;J4&amp;"*",D:D ))</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="L4" s="30" t="str">
-        <f t="shared" si="1"/>
-        <v>1:40</v>
-      </c>
-      <c r="M4" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>20%</v>
+        <v>0:00</v>
+      </c>
+      <c r="M4" s="11" t="str">
+        <f>ROUND((K4) / ($K$6), 2) * 100 &amp;"%"</f>
+        <v>0%</v>
       </c>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="6"/>
+    <row r="5" spans="1:19" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="6">
+        <v>5</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="17">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="L5" s="30" t="str">
-        <f t="shared" si="1"/>
-        <v>1:40</v>
-      </c>
-      <c r="M5" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>20%</v>
+        <v>12</v>
+      </c>
+      <c r="K5" s="14">
+        <f>SUMIFS(D:D,B:B, "&lt;&gt;*"&amp;J2&amp;"*",B:B, "&lt;&gt;*"&amp;#REF!&amp;"*",B:B, "&lt;&gt;*"&amp;J3&amp;"*",B:B, "&lt;&gt;*"&amp;J4&amp;"*")</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="25" t="str">
+        <f>ROUNDDOWN((K5)/60,0) &amp;":"&amp;(IF(MOD(K5, 60) &lt; 10, "0","")) &amp; MOD(K5,60)</f>
+        <v>0:00</v>
+      </c>
+      <c r="M5" s="11" t="str">
+        <f>ROUND((K5) / ($K$6), 2) * 100 &amp;"%"</f>
+        <v>0%</v>
       </c>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:19" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="6"/>
+    <row r="6" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="6">
+        <v>20</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="10"/>
+      <c r="H6" s="9"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="15">
-        <f>SUMIFS(D:D,B:B, "&lt;&gt;*"&amp;J2&amp;"*",B:B, "&lt;&gt;*"&amp;J3&amp;"*",B:B, "&lt;&gt;*"&amp;J4&amp;"*",B:B, "&lt;&gt;*"&amp;J5&amp;"*")</f>
-        <v>100</v>
-      </c>
-      <c r="L6" s="30" t="str">
+      <c r="K6" s="10">
+        <f>SUM(K2:K4) + K5</f>
+        <v>598</v>
+      </c>
+      <c r="L6" s="25" t="str">
         <f>ROUNDDOWN((K6)/60,0) &amp;":"&amp;(IF(MOD(K6, 60) &lt; 10, "0","")) &amp; MOD(K6,60)</f>
-        <v>1:40</v>
-      </c>
-      <c r="M6" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>20%</v>
-      </c>
+        <v>9:58</v>
+      </c>
+      <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:19" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="29"/>
+    <row r="7" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="11">
-        <f>SUM(K2:K5) + K6</f>
-        <v>500</v>
-      </c>
-      <c r="L7" s="30" t="str">
-        <f>ROUNDDOWN((K7)/60,0) &amp;":"&amp;(IF(MOD(K7, 60) &lt; 10, "0","")) &amp; MOD(K7,60)</f>
-        <v>8:20</v>
-      </c>
-      <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
+    </row>
+    <row r="8" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="20"/>
+      <c r="D15" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="20"/>
+      <c r="D18" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="20"/>
+      <c r="D19" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="20"/>
+      <c r="D21" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="20"/>
+      <c r="D22" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="20"/>
+      <c r="D23" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="D24" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="20"/>
+      <c r="D26" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="20"/>
+      <c r="D27" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="20"/>
+      <c r="D28" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="20"/>
+      <c r="D30" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="20"/>
+      <c r="D31" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="20"/>
+      <c r="D32" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="20"/>
+      <c r="D33" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="20"/>
+      <c r="D34" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="20"/>
+      <c r="D35" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="20"/>
+      <c r="D36" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="20"/>
+      <c r="D37" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="20"/>
+      <c r="D38" s="6"/>
+    </row>
+    <row r="39" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="20"/>
+      <c r="D40" s="6"/>
+    </row>
+    <row r="41" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="20"/>
+      <c r="D41" s="6"/>
+    </row>
+    <row r="42" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="20"/>
+      <c r="D42" s="6"/>
+    </row>
+    <row r="43" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="6"/>
+    </row>
+    <row r="45" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="6"/>
+    </row>
+    <row r="46" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="6"/>
+    </row>
+    <row r="47" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="6"/>
+    </row>
+    <row r="48" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tasks for Georgi week1 - week5
</commit_message>
<xml_diff>
--- a/Deliverables/Tasks.xlsx
+++ b/Deliverables/Tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
@@ -11,22 +11,16 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
-  <si>
-    <t>Tasks waiting to be completed:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
   <si>
     <t>Worked by:</t>
   </si>
   <si>
-    <t>Date and hour started</t>
-  </si>
-  <si>
     <t>Minutes worked</t>
   </si>
   <si>
@@ -54,9 +48,6 @@
     <t>Completed</t>
   </si>
   <si>
-    <t>Group</t>
-  </si>
-  <si>
     <t>as a Group</t>
   </si>
   <si>
@@ -72,23 +63,140 @@
     <t>Daniel</t>
   </si>
   <si>
-    <t>Something</t>
-  </si>
-  <si>
-    <t>Georgi  Ilia  Yu  Daniel</t>
-  </si>
-  <si>
-    <t>dd.mm. || hh:mm</t>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Wireframes</t>
+  </si>
+  <si>
+    <t>Yu and Georgi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date </t>
+  </si>
+  <si>
+    <t>17/11</t>
+  </si>
+  <si>
+    <t>User Interface</t>
+  </si>
+  <si>
+    <t>20/11</t>
+  </si>
+  <si>
+    <t>Part of use cases</t>
+  </si>
+  <si>
+    <t>19/11</t>
+  </si>
+  <si>
+    <t>Non func requirements</t>
+  </si>
+  <si>
+    <t>Georgi and Yu</t>
+  </si>
+  <si>
+    <t>Week 2</t>
+  </si>
+  <si>
+    <t>Fix URS mistakes</t>
+  </si>
+  <si>
+    <t>24/11</t>
+  </si>
+  <si>
+    <t>Class diagram v1</t>
+  </si>
+  <si>
+    <t>Georgi and Ilia</t>
+  </si>
+  <si>
+    <t>25/11</t>
+  </si>
+  <si>
+    <t>URS final</t>
+  </si>
+  <si>
+    <t>Yu Ilia and Georgi</t>
+  </si>
+  <si>
+    <t>26/11</t>
+  </si>
+  <si>
+    <t>Class diagram v2</t>
+  </si>
+  <si>
+    <t>Ilia and Georgi</t>
+  </si>
+  <si>
+    <t>27/11</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>Sequence diagram: Add element</t>
+  </si>
+  <si>
+    <t>Introduction to design doc</t>
+  </si>
+  <si>
+    <t>02/12</t>
+  </si>
+  <si>
+    <t>03/12</t>
+  </si>
+  <si>
+    <t>Create element icons</t>
+  </si>
+  <si>
+    <t>Icon below cursor</t>
+  </si>
+  <si>
+    <t>04/12</t>
+  </si>
+  <si>
+    <t>06/12</t>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>ConnectionZone coordinates</t>
+  </si>
+  <si>
+    <t>08/12</t>
+  </si>
+  <si>
+    <t>ConnectionZone states</t>
+  </si>
+  <si>
+    <t>11/12</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Flow visualization</t>
+  </si>
+  <si>
+    <t>16/12</t>
+  </si>
+  <si>
+    <t>Flow angle adjustment</t>
+  </si>
+  <si>
+    <t>18/12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm\.dd\.\ \|\|\ hh:mm"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,7 +261,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -398,40 +506,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="mediumDashed">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="mediumDashed">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -506,25 +586,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="1" builtinId="10"/>
+    <cellStyle name="Бележка" xfId="1" builtinId="10"/>
+    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -537,9 +611,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office тема">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Оffice">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -577,7 +651,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Оffice">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -611,7 +685,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -646,10 +719,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Оffice">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -822,14 +894,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="26.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="33.85546875" customWidth="1"/>
@@ -840,34 +912,34 @@
     <col min="11" max="11" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="26.25" customHeight="1" thickBot="1">
       <c r="A1" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="C1" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="25" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>3</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="20" t="s">
         <v>5</v>
-      </c>
-      <c r="K1" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="20" t="s">
-        <v>7</v>
       </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -877,138 +949,154 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="26.25" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>20</v>
-      </c>
       <c r="D2" s="6">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K2" s="17">
         <f>(SUMIF(B:B, "*"&amp;J2&amp;"*",D:D ))</f>
-        <v>100</v>
-      </c>
-      <c r="L2" s="30" t="str">
+        <v>1110</v>
+      </c>
+      <c r="L2" s="26" t="str">
         <f>ROUNDDOWN((K2)/60,0) &amp;":"&amp;(IF(MOD(K2, 60) &lt; 10, "0","")) &amp; MOD(K2,60)</f>
-        <v>1:40</v>
+        <v>18:30</v>
       </c>
       <c r="M2" s="12" t="str">
         <f>ROUND((K2) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>20%</v>
+        <v>71%</v>
       </c>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="26.25" customHeight="1">
       <c r="A3" s="6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="6">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K3" s="17">
-        <f t="shared" ref="K3:K5" si="0">(SUMIF(B:B, "*"&amp;J3&amp;"*",D:D ))</f>
-        <v>100</v>
-      </c>
-      <c r="L3" s="30" t="str">
-        <f t="shared" ref="L3:L5" si="1">ROUNDDOWN((K3)/60,0) &amp;":"&amp;(IF(MOD(K3, 60) &lt; 10, "0","")) &amp; MOD(K3,60)</f>
-        <v>1:40</v>
+        <f>(SUMIF(B:B, "*"&amp;J3&amp;"*",D:D ))</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="26" t="str">
+        <f>ROUNDDOWN((K3)/60,0) &amp;":"&amp;(IF(MOD(K3, 60) &lt; 10, "0","")) &amp; MOD(K3,60)</f>
+        <v>0:00</v>
       </c>
       <c r="M3" s="12" t="str">
-        <f t="shared" ref="M3:M6" si="2">ROUND((K3) / ($K$7), 2) * 100 &amp;"%"</f>
-        <v>20%</v>
+        <f>ROUND((K3) / ($K$7), 2) * 100 &amp;"%"</f>
+        <v>0%</v>
       </c>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="6"/>
+    <row r="4" spans="1:19" ht="26.25" customHeight="1">
+      <c r="A4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="6">
+        <v>40</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="9"/>
       <c r="I4" s="1"/>
       <c r="J4" s="13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K4" s="17">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="L4" s="30" t="str">
-        <f t="shared" si="1"/>
-        <v>1:40</v>
+        <f t="shared" ref="K4:K5" si="0">(SUMIF(B:B, "*"&amp;J4&amp;"*",D:D ))</f>
+        <v>240</v>
+      </c>
+      <c r="L4" s="26" t="str">
+        <f t="shared" ref="L4:L5" si="1">ROUNDDOWN((K4)/60,0) &amp;":"&amp;(IF(MOD(K4, 60) &lt; 10, "0","")) &amp; MOD(K4,60)</f>
+        <v>4:00</v>
       </c>
       <c r="M4" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>20%</v>
+        <f t="shared" ref="M4:M6" si="2">ROUND((K4) / ($K$7), 2) * 100 &amp;"%"</f>
+        <v>15%</v>
       </c>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="6"/>
+    <row r="5" spans="1:19" ht="26.25" customHeight="1">
+      <c r="A5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="6">
+        <v>30</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K5" s="17">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="L5" s="30" t="str">
+        <v>220</v>
+      </c>
+      <c r="L5" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>1:40</v>
+        <v>3:40</v>
       </c>
       <c r="M5" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>20%</v>
+        <v>14%</v>
       </c>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:19" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
+    <row r="6" spans="1:19" ht="26.25" customHeight="1" thickBot="1">
+      <c r="A6" s="7"/>
       <c r="B6" s="8"/>
       <c r="C6" s="21"/>
       <c r="D6" s="6"/>
@@ -1018,42 +1106,42 @@
       <c r="H6" s="10"/>
       <c r="I6" s="1"/>
       <c r="J6" s="14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="K6" s="15">
         <f>SUMIFS(D:D,B:B, "&lt;&gt;*"&amp;J2&amp;"*",B:B, "&lt;&gt;*"&amp;J3&amp;"*",B:B, "&lt;&gt;*"&amp;J4&amp;"*",B:B, "&lt;&gt;*"&amp;J5&amp;"*")</f>
-        <v>100</v>
-      </c>
-      <c r="L6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="L6" s="26" t="str">
         <f>ROUNDDOWN((K6)/60,0) &amp;":"&amp;(IF(MOD(K6, 60) &lt; 10, "0","")) &amp; MOD(K6,60)</f>
-        <v>1:40</v>
+        <v>0:00</v>
       </c>
       <c r="M6" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>20%</v>
+        <v>0%</v>
       </c>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:19" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="29"/>
+    <row r="7" spans="1:19" ht="26.25" customHeight="1">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K7" s="11">
         <f>SUM(K2:K5) + K6</f>
-        <v>500</v>
-      </c>
-      <c r="L7" s="30" t="str">
+        <v>1570</v>
+      </c>
+      <c r="L7" s="26" t="str">
         <f>ROUNDDOWN((K7)/60,0) &amp;":"&amp;(IF(MOD(K7, 60) &lt; 10, "0","")) &amp; MOD(K7,60)</f>
-        <v>8:20</v>
+        <v>26:10</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -1063,30 +1151,234 @@
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
     </row>
+    <row r="8" spans="1:19" ht="26.25" customHeight="1">
+      <c r="A8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="6">
+        <v>30</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="26.25" customHeight="1">
+      <c r="A9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="26.25" customHeight="1">
+      <c r="A10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="26.25" customHeight="1">
+      <c r="A11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="26.25" customHeight="1">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:19" ht="26.25" customHeight="1">
+      <c r="A13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="6">
+        <v>60</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="26.25" customHeight="1">
+      <c r="A14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="26.25" customHeight="1">
+      <c r="A15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="26.25" customHeight="1">
+      <c r="A16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="26.25" customHeight="1">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" ht="26.25" customHeight="1">
+      <c r="A18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="6">
+        <v>20</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="26.25" customHeight="1">
+      <c r="A19" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="26.25" customHeight="1">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="1:5" ht="26.25" customHeight="1">
+      <c r="A21" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="6">
+        <v>120</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="26.25" customHeight="1">
+      <c r="A22" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="6">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="26.25" customHeight="1">
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Tasks added dates and hours
</commit_message>
<xml_diff>
--- a/Deliverables/Tasks.xlsx
+++ b/Deliverables/Tasks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="127">
   <si>
     <t>Worked by:</t>
   </si>
@@ -285,9 +285,6 @@
     <t>App: Flow angle adjustment</t>
   </si>
   <si>
-    <t>30.12 || 13:00</t>
-  </si>
-  <si>
     <t>App: Information box</t>
   </si>
   <si>
@@ -307,6 +304,99 @@
   </si>
   <si>
     <t>02.01. || 11:30</t>
+  </si>
+  <si>
+    <t>29.12 || 12:00</t>
+  </si>
+  <si>
+    <t>22.12 || 12:00</t>
+  </si>
+  <si>
+    <t>15.12 || 13:00</t>
+  </si>
+  <si>
+    <t>10.12. || 13:00</t>
+  </si>
+  <si>
+    <t>11.12. || 13:02</t>
+  </si>
+  <si>
+    <t>10.12. || 13:20</t>
+  </si>
+  <si>
+    <t>13.12 || 15:00</t>
+  </si>
+  <si>
+    <t>13.12 || 15:05</t>
+  </si>
+  <si>
+    <t>13.12 || 15:10</t>
+  </si>
+  <si>
+    <t>13.12 || 15:15</t>
+  </si>
+  <si>
+    <t>Georgi and Yu</t>
+  </si>
+  <si>
+    <t>16.12 || 14:00</t>
+  </si>
+  <si>
+    <t>18.12 || 13:00</t>
+  </si>
+  <si>
+    <t>19.12 || 13:00</t>
+  </si>
+  <si>
+    <t>19.12 || 13:15</t>
+  </si>
+  <si>
+    <t>22.12 || 12:30</t>
+  </si>
+  <si>
+    <t>22.12 || 12:38</t>
+  </si>
+  <si>
+    <t>28.12 || 15:00</t>
+  </si>
+  <si>
+    <t>28.12 || 15:10</t>
+  </si>
+  <si>
+    <t>22.12 || 12:58</t>
+  </si>
+  <si>
+    <t>22.12 || 13:03</t>
+  </si>
+  <si>
+    <t>22.12 || 13:00</t>
+  </si>
+  <si>
+    <t>25.12 || 16:00</t>
+  </si>
+  <si>
+    <t>27.12 || 18:00</t>
+  </si>
+  <si>
+    <t>30.12. || 14:00</t>
+  </si>
+  <si>
+    <t>30.12. || 14:10</t>
+  </si>
+  <si>
+    <t>30.12. || 14:20</t>
+  </si>
+  <si>
+    <t>30.12. || 14:25</t>
+  </si>
+  <si>
+    <t>30.12 || 15:00</t>
+  </si>
+  <si>
+    <t>30.12 || 16:00</t>
+  </si>
+  <si>
+    <t>30.12 || 17:00</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1102,7 @@
   <dimension ref="A1:M56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" customHeight="1"/>
@@ -1087,7 +1177,7 @@
       </c>
       <c r="M2" s="12" t="str">
         <f>ROUND((K2) / ($K$6), 2) * 100 &amp;"%"</f>
-        <v>52%</v>
+        <v>49%</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="26.25" customHeight="1">
@@ -1103,6 +1193,7 @@
       <c r="D3" s="6">
         <v>40</v>
       </c>
+      <c r="E3" s="2"/>
       <c r="H3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1119,7 +1210,7 @@
       </c>
       <c r="M3" s="12" t="str">
         <f>ROUND((K3) / ($K$6), 2) * 100 &amp;"%"</f>
-        <v>46%</v>
+        <v>44%</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="26.25" customHeight="1">
@@ -1135,21 +1226,22 @@
       <c r="D4" s="6">
         <v>20</v>
       </c>
+      <c r="E4" s="2"/>
       <c r="H4" s="9"/>
       <c r="J4" s="13" t="s">
         <v>12</v>
       </c>
       <c r="K4" s="17">
         <f>(SUMIF(B:B, "*"&amp;J4&amp;"*",D:D ))</f>
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="L4" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>0:30</v>
+        <v>1:20</v>
       </c>
       <c r="M4" s="12" t="str">
         <f>ROUND((K4) / ($K$6), 2) * 100 &amp;"%"</f>
-        <v>3%</v>
+        <v>7%</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="26.25" customHeight="1" thickBot="1">
@@ -1157,7 +1249,7 @@
         <v>29</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>30</v>
@@ -1165,6 +1257,7 @@
       <c r="D5" s="6">
         <v>20</v>
       </c>
+      <c r="E5" s="2"/>
       <c r="J5" s="14" t="s">
         <v>10</v>
       </c>
@@ -1194,17 +1287,18 @@
       <c r="D6" s="6">
         <v>5</v>
       </c>
+      <c r="E6" s="2"/>
       <c r="H6" s="10"/>
       <c r="J6" s="13" t="s">
         <v>11</v>
       </c>
       <c r="K6" s="11">
         <f>SUM(K2:K4) + K5</f>
-        <v>1123</v>
+        <v>1173</v>
       </c>
       <c r="L6" s="26" t="str">
         <f>ROUNDDOWN((K6)/60,0) &amp;":"&amp;(IF(MOD(K6, 60) &lt; 10, "0","")) &amp; MOD(K6,60)</f>
-        <v>18:43</v>
+        <v>19:33</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="26.25" customHeight="1">
@@ -1212,7 +1306,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>33</v>
@@ -1220,7 +1314,7 @@
       <c r="D7" s="6">
         <v>30</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1237,6 +1331,7 @@
       <c r="D8" s="6">
         <v>20</v>
       </c>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:13" ht="26.25" customHeight="1">
       <c r="A9" s="6" t="s">
@@ -1251,6 +1346,7 @@
       <c r="D9" s="6">
         <v>5</v>
       </c>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:13" ht="26.25" customHeight="1">
       <c r="A10" s="6" t="s">
@@ -1265,6 +1361,7 @@
       <c r="D10" s="6">
         <v>40</v>
       </c>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:13" ht="26.25" customHeight="1">
       <c r="A11" s="6" t="s">
@@ -1279,6 +1376,7 @@
       <c r="D11" s="6">
         <v>10</v>
       </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:13" ht="26.25" customHeight="1">
       <c r="A12" s="6" t="s">
@@ -1293,7 +1391,7 @@
       <c r="D12" s="6">
         <v>10</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1310,6 +1408,7 @@
       <c r="D13" s="6">
         <v>20</v>
       </c>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:13" ht="26.25" customHeight="1">
       <c r="A14" s="6" t="s">
@@ -1324,6 +1423,7 @@
       <c r="D14" s="6">
         <v>30</v>
       </c>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:13" ht="26.25" customHeight="1">
       <c r="A15" s="6" t="s">
@@ -1338,6 +1438,7 @@
       <c r="D15" s="6">
         <v>60</v>
       </c>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:13" ht="26.25" customHeight="1">
       <c r="A16" s="6" t="s">
@@ -1352,6 +1453,7 @@
       <c r="D16" s="6">
         <v>30</v>
       </c>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" ht="26.25" customHeight="1">
       <c r="A17" s="6" t="s">
@@ -1366,6 +1468,7 @@
       <c r="D17" s="6">
         <v>30</v>
       </c>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" ht="26.25" customHeight="1">
       <c r="A18" s="6" t="s">
@@ -1380,6 +1483,9 @@
       <c r="D18" s="6">
         <v>10</v>
       </c>
+      <c r="E18" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="26.25" customHeight="1">
       <c r="A19" s="6" t="s">
@@ -1388,13 +1494,13 @@
       <c r="B19" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="21"/>
+      <c r="C19" s="21" t="s">
+        <v>99</v>
+      </c>
       <c r="D19" s="6">
         <v>20</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" ht="26.25" customHeight="1">
       <c r="A20" s="6" t="s">
@@ -1403,10 +1509,13 @@
       <c r="B20" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="21"/>
+      <c r="C20" s="21" t="s">
+        <v>101</v>
+      </c>
       <c r="D20" s="6">
         <v>40</v>
       </c>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" ht="26.25" customHeight="1">
       <c r="A21" s="6" t="s">
@@ -1415,10 +1524,13 @@
       <c r="B21" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="21"/>
+      <c r="C21" s="21" t="s">
+        <v>100</v>
+      </c>
       <c r="D21" s="6">
         <v>10</v>
       </c>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" ht="26.25" customHeight="1">
       <c r="A22" s="6" t="s">
@@ -1427,10 +1539,13 @@
       <c r="B22" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="21"/>
+      <c r="C22" s="21" t="s">
+        <v>102</v>
+      </c>
       <c r="D22" s="6">
         <v>5</v>
       </c>
+      <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" ht="26.25" customHeight="1">
       <c r="A23" s="6" t="s">
@@ -1439,10 +1554,13 @@
       <c r="B23" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="21"/>
+      <c r="C23" s="21" t="s">
+        <v>103</v>
+      </c>
       <c r="D23" s="6">
         <v>5</v>
       </c>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" ht="26.25" customHeight="1">
       <c r="A24" s="6" t="s">
@@ -1451,10 +1569,13 @@
       <c r="B24" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="21"/>
+      <c r="C24" s="21" t="s">
+        <v>104</v>
+      </c>
       <c r="D24" s="6">
         <v>5</v>
       </c>
+      <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" ht="26.25" customHeight="1">
       <c r="A25" s="6" t="s">
@@ -1463,10 +1584,13 @@
       <c r="B25" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="21"/>
+      <c r="C25" s="21" t="s">
+        <v>105</v>
+      </c>
       <c r="D25" s="6">
         <v>5</v>
       </c>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" ht="26.25" customHeight="1">
       <c r="A26" s="6" t="s">
@@ -1475,11 +1599,13 @@
       <c r="B26" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="21"/>
+      <c r="C26" s="21" t="s">
+        <v>98</v>
+      </c>
       <c r="D26" s="6">
         <v>10</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1490,10 +1616,13 @@
       <c r="B27" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="21"/>
+      <c r="C27" s="21" t="s">
+        <v>107</v>
+      </c>
       <c r="D27" s="6">
         <v>5</v>
       </c>
+      <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" ht="26.25" customHeight="1">
       <c r="A28" s="6" t="s">
@@ -1502,10 +1631,13 @@
       <c r="B28" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="21"/>
+      <c r="C28" s="21" t="s">
+        <v>108</v>
+      </c>
       <c r="D28" s="6">
         <v>60</v>
       </c>
+      <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" ht="26.25" customHeight="1">
       <c r="A29" s="6" t="s">
@@ -1514,10 +1646,13 @@
       <c r="B29" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="21"/>
+      <c r="C29" s="21" t="s">
+        <v>109</v>
+      </c>
       <c r="D29" s="6">
         <v>5</v>
       </c>
+      <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" ht="26.25" customHeight="1">
       <c r="A30" s="6" t="s">
@@ -1526,10 +1661,13 @@
       <c r="B30" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="21"/>
+      <c r="C30" s="21" t="s">
+        <v>110</v>
+      </c>
       <c r="D30" s="6">
         <v>10</v>
       </c>
+      <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" ht="26.25" customHeight="1">
       <c r="A31" s="6" t="s">
@@ -1538,11 +1676,13 @@
       <c r="B31" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="21"/>
+      <c r="C31" s="21" t="s">
+        <v>97</v>
+      </c>
       <c r="D31" s="6">
         <v>30</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="2" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1553,10 +1693,13 @@
       <c r="B32" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="21"/>
+      <c r="C32" s="21" t="s">
+        <v>111</v>
+      </c>
       <c r="D32" s="6">
         <v>8</v>
       </c>
+      <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" ht="26.25" customHeight="1">
       <c r="A33" s="6" t="s">
@@ -1565,227 +1708,262 @@
       <c r="B33" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="21"/>
+      <c r="C33" s="21" t="s">
+        <v>112</v>
+      </c>
       <c r="D33" s="6">
         <v>20</v>
       </c>
+      <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5" ht="26.25" customHeight="1">
       <c r="A34" s="6" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="21"/>
-      <c r="D34" s="6">
-        <v>5</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="D34" s="6"/>
+      <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:5" ht="26.25" customHeight="1">
       <c r="A35" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="21"/>
+      <c r="C35" s="21" t="s">
+        <v>115</v>
+      </c>
       <c r="D35" s="6">
         <v>5</v>
       </c>
+      <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:5" ht="26.25" customHeight="1">
       <c r="A36" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="21"/>
+      <c r="C36" s="21" t="s">
+        <v>116</v>
+      </c>
       <c r="D36" s="6">
-        <v>10</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:5" ht="26.25" customHeight="1">
       <c r="A37" s="6" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="21"/>
-      <c r="D37" s="6">
-        <v>10</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5" ht="26.25" customHeight="1">
       <c r="A38" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="21"/>
+      <c r="C38" s="21" t="s">
+        <v>113</v>
+      </c>
       <c r="D38" s="6">
-        <v>20</v>
-      </c>
-      <c r="E38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="26.25" customHeight="1">
       <c r="A39" s="6" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="21"/>
-      <c r="D39" s="6">
-        <v>10</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39" s="6"/>
     </row>
     <row r="40" spans="1:5" ht="26.25" customHeight="1">
       <c r="A40" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="21"/>
+      <c r="C40" s="21" t="s">
+        <v>114</v>
+      </c>
       <c r="D40" s="6">
         <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="26.25" customHeight="1">
       <c r="A41" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="21"/>
+      <c r="C41" s="21" t="s">
+        <v>96</v>
+      </c>
       <c r="D41" s="6">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="26.25" customHeight="1">
       <c r="A42" s="6" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="21"/>
+        <v>7</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>87</v>
+      </c>
       <c r="D42" s="6">
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="26.25" customHeight="1">
       <c r="A43" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C43" s="21"/>
+        <v>8</v>
+      </c>
+      <c r="C43" s="21" t="s">
+        <v>120</v>
+      </c>
       <c r="D43" s="6">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="26.25" customHeight="1">
       <c r="A44" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="21"/>
+      <c r="C44" s="21" t="s">
+        <v>121</v>
+      </c>
       <c r="D44" s="6">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="26.25" customHeight="1">
       <c r="A45" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>87</v>
+        <v>122</v>
       </c>
       <c r="D45" s="6">
-        <v>60</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="26.25" customHeight="1">
       <c r="A46" s="6" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="D46" s="6">
-        <v>120</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="26.25" customHeight="1">
       <c r="A47" s="6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>91</v>
+        <v>124</v>
       </c>
       <c r="D47" s="6">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="26.25" customHeight="1">
       <c r="A48" s="6" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48" s="21"/>
-      <c r="D48" s="6"/>
+        <v>8</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D48" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="49" spans="1:4" ht="26.25" customHeight="1">
       <c r="A49" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49" s="21"/>
-      <c r="D49" s="6"/>
+        <v>7</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D49" s="6">
+        <v>120</v>
+      </c>
     </row>
     <row r="50" spans="1:4" ht="26.25" customHeight="1">
       <c r="A50" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C50" s="21"/>
-      <c r="D50" s="6"/>
+        <v>8</v>
+      </c>
+      <c r="C50" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D50" s="6">
+        <v>10</v>
+      </c>
     </row>
     <row r="51" spans="1:4" ht="26.25" customHeight="1">
       <c r="A51" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="21" t="s">
         <v>95</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51" s="21" t="s">
-        <v>96</v>
       </c>
       <c r="D51" s="6">
         <v>30</v>

</xml_diff>